<commit_message>
2025-06-04 LeetCode Sum Multiples
</commit_message>
<xml_diff>
--- a/plans/30_day_easy_dsa_schedule.xlsx
+++ b/plans/30_day_easy_dsa_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annimukh/code/2_dsa/plans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762BFA40-E4DF-7743-8D0A-817F481A17E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D3CC06-886A-1D45-9E55-DC9CBD5D8546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="900" windowWidth="41080" windowHeight="25000" xr2:uid="{28D46363-2EB7-6B4C-B566-6834E9168DA2}"/>
   </bookViews>
@@ -1490,13 +1490,13 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>